<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758104150727_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758104150727_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758104150727_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B591AF90-ADE9-4E6D-9304-4B13108D19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10575" windowHeight="7830"/>
+    <workbookView xWindow="1520" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -273,9 +274,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -310,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,27 +650,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -682,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -690,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D2" s="2">
         <v>0.48604166666666665</v>
@@ -702,7 +703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -710,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D3" s="3">
         <v>0.48604166666666665</v>
@@ -722,7 +723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -730,7 +731,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D4" s="3">
         <v>0.48604166666666665</v>
@@ -742,7 +743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -750,7 +751,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D5" s="3">
         <v>0.48604166666666665</v>
@@ -762,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -770,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D6" s="3">
         <v>0.48604166666666665</v>
@@ -782,7 +783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -790,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D7" s="3">
         <v>0.48604166666666665</v>
@@ -802,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -810,7 +811,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D8" s="3">
         <v>0.48604166666666665</v>
@@ -822,7 +823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -830,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D9" s="3">
         <v>0.48604166666666665</v>
@@ -842,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -850,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D10" s="3">
         <v>0.48604166666666665</v>
@@ -862,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -870,7 +871,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D11" s="3">
         <v>0.48604166666666665</v>
@@ -882,7 +883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -890,7 +891,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D12" s="3">
         <v>0.48604166666666665</v>
@@ -902,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -910,7 +911,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D13" s="3">
         <v>0.48604166666666665</v>
@@ -922,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -930,7 +931,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D14" s="3">
         <v>0.48604166666666665</v>
@@ -942,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -950,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D15" s="3">
         <v>0.48604166666666665</v>
@@ -962,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -970,7 +971,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D16" s="3">
         <v>0.48604166666666665</v>
@@ -982,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -990,7 +991,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D17" s="3">
         <v>0.48604166666666665</v>
@@ -1002,7 +1003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D18" s="3">
         <v>0.48604166666666665</v>
@@ -1022,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D19" s="3">
         <v>0.48604166666666665</v>
@@ -1042,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D20" s="3">
         <v>0.48604166666666665</v>
@@ -1062,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1070,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D21" s="3">
         <v>0.48604166666666665</v>
@@ -1082,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D22" s="3">
         <v>0.48604166666666665</v>
@@ -1102,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D23" s="3">
         <v>0.48604166666666665</v>
@@ -1122,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D24" s="3">
         <v>0.48604166666666665</v>
@@ -1142,7 +1143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D25" s="3">
         <v>0.48604166666666665</v>
@@ -1162,7 +1163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D26" s="3">
         <v>0.48604166666666665</v>
@@ -1182,7 +1183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1190,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D27" s="3">
         <v>0.48604166666666665</v>
@@ -1202,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D28" s="3">
         <v>0.48604166666666665</v>
@@ -1222,7 +1223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D29" s="3">
         <v>0.48604166666666665</v>
@@ -1242,7 +1243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D30" s="3">
         <v>0.48604166666666665</v>
@@ -1262,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>7</v>
       </c>
       <c r="C31" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D31" s="3">
         <v>0.48604166666666665</v>
@@ -1282,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D32" s="3">
         <v>0.48604166666666665</v>
@@ -1302,7 +1303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D33" s="3">
         <v>0.48604166666666665</v>
@@ -1322,7 +1323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1330,7 +1331,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D34" s="3">
         <v>0.48604166666666665</v>
@@ -1342,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D35" s="3">
         <v>0.48604166666666665</v>
@@ -1362,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>7</v>
       </c>
       <c r="C36" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D36" s="3">
         <v>0.48604166666666665</v>
@@ -1382,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1390,7 +1391,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D37" s="3">
         <v>0.48604166666666665</v>
@@ -1402,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D38" s="3">
         <v>0.48604166666666665</v>
@@ -1422,7 +1423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D39" s="3">
         <v>0.48604166666666665</v>
@@ -1442,7 +1443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D40" s="3">
         <v>0.48604166666666665</v>
@@ -1462,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D41" s="3">
         <v>0.48604166666666665</v>
@@ -1482,7 +1483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -1490,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D42" s="3">
         <v>0.48604166666666665</v>
@@ -1502,7 +1503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>7</v>
       </c>
       <c r="C43" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D43" s="3">
         <v>0.48604166666666665</v>
@@ -1522,7 +1523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>7</v>
       </c>
       <c r="C44" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D44" s="3">
         <v>0.48604166666666665</v>
@@ -1542,7 +1543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>7</v>
       </c>
       <c r="C45" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D45" s="3">
         <v>0.48604166666666665</v>
@@ -1562,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D46" s="3">
         <v>0.48604166666666665</v>
@@ -1582,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D47" s="3">
         <v>0.48604166666666665</v>
@@ -1602,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D48" s="3">
         <v>0.48604166666666665</v>
@@ -1622,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D49" s="3">
         <v>0.48604166666666665</v>
@@ -1642,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D50" s="3">
         <v>0.48604166666666665</v>
@@ -1662,7 +1663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D51" s="3">
         <v>0.48604166666666665</v>
@@ -1682,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D52" s="3">
         <v>0.48604166666666665</v>
@@ -1702,7 +1703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -1710,7 +1711,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D53" s="3">
         <v>0.48604166666666665</v>
@@ -1722,7 +1723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D54" s="3">
         <v>0.48604166666666665</v>
@@ -1742,7 +1743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>7</v>
       </c>
       <c r="C55" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D55" s="3">
         <v>0.48604166666666665</v>
@@ -1762,7 +1763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D56" s="3">
         <v>0.48604166666666665</v>
@@ -1782,7 +1783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D57" s="3">
         <v>0.48604166666666665</v>
@@ -1802,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -1810,7 +1811,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D58" s="3">
         <v>0.48604166666666665</v>
@@ -1822,7 +1823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -1830,7 +1831,7 @@
         <v>7</v>
       </c>
       <c r="C59" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D59" s="3">
         <v>0.48604166666666665</v>
@@ -1842,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>7</v>
       </c>
       <c r="C60" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D60" s="3">
         <v>0.48604166666666665</v>
@@ -1862,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -1870,7 +1871,7 @@
         <v>7</v>
       </c>
       <c r="C61" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D61" s="3">
         <v>0.48604166666666665</v>
@@ -1882,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -1890,7 +1891,7 @@
         <v>7</v>
       </c>
       <c r="C62" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D62" s="3">
         <v>0.48604166666666665</v>
@@ -1902,7 +1903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -1910,7 +1911,7 @@
         <v>7</v>
       </c>
       <c r="C63" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D63" s="3">
         <v>0.48604166666666665</v>
@@ -1922,7 +1923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D64" s="3">
         <v>0.48604166666666665</v>
@@ -1942,7 +1943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D65" s="3">
         <v>0.48604166666666665</v>
@@ -1962,7 +1963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D66" s="3">
         <v>0.48604166666666665</v>
@@ -1982,7 +1983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>7</v>
       </c>
       <c r="C67" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D67" s="3">
         <v>0.48604166666666665</v>
@@ -2002,7 +2003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>7</v>
       </c>
       <c r="C68" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D68" s="3">
         <v>0.48604166666666665</v>
@@ -2022,7 +2023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -2030,7 +2031,7 @@
         <v>7</v>
       </c>
       <c r="C69" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D69" s="3">
         <v>0.48604166666666665</v>
@@ -2042,7 +2043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2050,7 +2051,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D70" s="3">
         <v>0.48604166666666665</v>
@@ -2062,7 +2063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>7</v>
       </c>
       <c r="C71" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D71" s="3">
         <v>0.48604166666666665</v>
@@ -2082,7 +2083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -2090,7 +2091,7 @@
         <v>7</v>
       </c>
       <c r="C72" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D72" s="3">
         <v>0.48604166666666665</v>
@@ -2102,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>7</v>
       </c>
       <c r="C73" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D73" s="3">
         <v>0.48604166666666665</v>
@@ -2122,7 +2123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -2130,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="C74" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D74" s="3">
         <v>0.48604166666666665</v>
@@ -2142,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -2150,7 +2151,7 @@
         <v>7</v>
       </c>
       <c r="C75" s="1">
-        <v>45847</v>
+        <v>45907</v>
       </c>
       <c r="D75" s="3">
         <v>0.48604166666666665</v>

</xml_diff>